<commit_message>
replace example data sets with real ones
</commit_message>
<xml_diff>
--- a/inst/extdata/tecan_time_series_multiple_reads.xlsx
+++ b/inst/extdata/tecan_time_series_multiple_reads.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11110"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gleb/polybox/PhD/Bioinformatics/Rpackages/tecanr/inst/extdata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gleb/polybox/PhD/Science/Software/tecanr/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7F16C88-6EE3-024E-8C2F-046C800429CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB6A4A2D-958D-9741-BC0A-22C5BEC3BD06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22400" yWindow="12860" windowWidth="22400" windowHeight="12340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19200" yWindow="500" windowWidth="19200" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -1516,10 +1516,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U130"/>
+  <dimension ref="A1:Z130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:XFD17"/>
+    <sheetView tabSelected="1" topLeftCell="Q87" workbookViewId="0">
+      <selection activeCell="Z115" sqref="Z115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1836,12 +1836,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="56" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="57" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A57" s="5" t="s">
         <v>40</v>
       </c>
@@ -1905,8 +1905,23 @@
       <c r="U57" s="5">
         <v>20</v>
       </c>
-    </row>
-    <row r="58" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V57" s="5">
+        <v>21</v>
+      </c>
+      <c r="W57" s="5">
+        <v>22</v>
+      </c>
+      <c r="X57" s="5">
+        <v>23</v>
+      </c>
+      <c r="Y57" s="5">
+        <v>24</v>
+      </c>
+      <c r="Z57" s="5">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="58" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A58" s="5" t="s">
         <v>41</v>
       </c>
@@ -1971,7 +1986,7 @@
         <v>11400.1</v>
       </c>
     </row>
-    <row r="59" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A59" s="5" t="s">
         <v>42</v>
       </c>
@@ -2036,7 +2051,7 @@
         <v>31.2</v>
       </c>
     </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A60" s="5" t="s">
         <v>43</v>
       </c>
@@ -2101,7 +2116,7 @@
         <v>9.8200000822544098E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A61" s="5" t="s">
         <v>44</v>
       </c>
@@ -2166,7 +2181,7 @@
         <v>1.3700000010430813E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A62" s="5" t="s">
         <v>45</v>
       </c>
@@ -2231,7 +2246,7 @@
         <v>9.1399997472763062E-2</v>
       </c>
     </row>
-    <row r="63" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A63" s="5" t="s">
         <v>46</v>
       </c>
@@ -2296,7 +2311,7 @@
         <v>0.12229999899864197</v>
       </c>
     </row>
-    <row r="64" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A64" s="5" t="s">
         <v>47</v>
       </c>
@@ -2361,7 +2376,7 @@
         <v>8.9900001883506775E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A65" s="5" t="s">
         <v>48</v>
       </c>
@@ -2426,7 +2441,7 @@
         <v>9.6000000834465027E-2</v>
       </c>
     </row>
-    <row r="66" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A66" s="5" t="s">
         <v>49</v>
       </c>
@@ -2491,12 +2506,12 @@
         <v>9.1399997472763062E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="69" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A69" s="5" t="s">
         <v>50</v>
       </c>
@@ -2560,8 +2575,23 @@
       <c r="U69" s="5">
         <v>20</v>
       </c>
-    </row>
-    <row r="70" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V69" s="5">
+        <v>21</v>
+      </c>
+      <c r="W69" s="5">
+        <v>22</v>
+      </c>
+      <c r="X69" s="5">
+        <v>23</v>
+      </c>
+      <c r="Y69" s="5">
+        <v>24</v>
+      </c>
+      <c r="Z69" s="5">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="70" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A70" s="5" t="s">
         <v>41</v>
       </c>
@@ -2626,7 +2656,7 @@
         <v>11400.1</v>
       </c>
     </row>
-    <row r="71" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A71" s="5" t="s">
         <v>42</v>
       </c>
@@ -2691,7 +2721,7 @@
         <v>31.2</v>
       </c>
     </row>
-    <row r="72" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A72" s="5" t="s">
         <v>43</v>
       </c>
@@ -2756,7 +2786,7 @@
         <v>9.9299997091293335E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A73" s="5" t="s">
         <v>44</v>
       </c>
@@ -2821,7 +2851,7 @@
         <v>1.2799999676644802E-2</v>
       </c>
     </row>
-    <row r="74" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A74" s="5" t="s">
         <v>45</v>
       </c>
@@ -2886,7 +2916,7 @@
         <v>9.3299999833106995E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A75" s="5" t="s">
         <v>46</v>
       </c>
@@ -2951,7 +2981,7 @@
         <v>0.12099999934434891</v>
       </c>
     </row>
-    <row r="76" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A76" s="5" t="s">
         <v>47</v>
       </c>
@@ -3016,7 +3046,7 @@
         <v>8.9100003242492676E-2</v>
       </c>
     </row>
-    <row r="77" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A77" s="5" t="s">
         <v>48</v>
       </c>
@@ -3081,7 +3111,7 @@
         <v>0.1005999967455864</v>
       </c>
     </row>
-    <row r="78" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A78" s="5" t="s">
         <v>49</v>
       </c>
@@ -3146,12 +3176,12 @@
         <v>9.2299997806549072E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="81" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A81" s="5" t="s">
         <v>51</v>
       </c>
@@ -3215,8 +3245,23 @@
       <c r="U81" s="5">
         <v>20</v>
       </c>
-    </row>
-    <row r="82" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V81" s="5">
+        <v>21</v>
+      </c>
+      <c r="W81" s="5">
+        <v>22</v>
+      </c>
+      <c r="X81" s="5">
+        <v>23</v>
+      </c>
+      <c r="Y81" s="5">
+        <v>24</v>
+      </c>
+      <c r="Z81" s="5">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="82" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A82" s="5" t="s">
         <v>41</v>
       </c>
@@ -3281,7 +3326,7 @@
         <v>11400.1</v>
       </c>
     </row>
-    <row r="83" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A83" s="5" t="s">
         <v>42</v>
       </c>
@@ -3346,7 +3391,7 @@
         <v>31.2</v>
       </c>
     </row>
-    <row r="84" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A84" s="5" t="s">
         <v>43</v>
       </c>
@@ -3411,7 +3456,7 @@
         <v>0.10149999707937241</v>
       </c>
     </row>
-    <row r="85" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A85" s="5" t="s">
         <v>44</v>
       </c>
@@ -3476,7 +3521,7 @@
         <v>1.4499999582767487E-2</v>
       </c>
     </row>
-    <row r="86" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A86" s="5" t="s">
         <v>45</v>
       </c>
@@ -3541,7 +3586,7 @@
         <v>9.7099997103214264E-2</v>
       </c>
     </row>
-    <row r="87" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A87" s="5" t="s">
         <v>46</v>
       </c>
@@ -3606,7 +3651,7 @@
         <v>0.1265999972820282</v>
       </c>
     </row>
-    <row r="88" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A88" s="5" t="s">
         <v>47</v>
       </c>
@@ -3671,7 +3716,7 @@
         <v>9.0599998831748962E-2</v>
       </c>
     </row>
-    <row r="89" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A89" s="5" t="s">
         <v>48</v>
       </c>
@@ -3736,7 +3781,7 @@
         <v>9.9799998104572296E-2</v>
       </c>
     </row>
-    <row r="90" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A90" s="5" t="s">
         <v>49</v>
       </c>
@@ -3801,12 +3846,12 @@
         <v>9.3400001525878906E-2</v>
       </c>
     </row>
-    <row r="92" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="93" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A93" s="5" t="s">
         <v>52</v>
       </c>
@@ -3870,8 +3915,23 @@
       <c r="U93" s="5">
         <v>20</v>
       </c>
-    </row>
-    <row r="94" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V93" s="5">
+        <v>21</v>
+      </c>
+      <c r="W93" s="5">
+        <v>22</v>
+      </c>
+      <c r="X93" s="5">
+        <v>23</v>
+      </c>
+      <c r="Y93" s="5">
+        <v>24</v>
+      </c>
+      <c r="Z93" s="5">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="94" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A94" s="5" t="s">
         <v>41</v>
       </c>
@@ -3936,7 +3996,7 @@
         <v>11400.1</v>
       </c>
     </row>
-    <row r="95" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A95" s="5" t="s">
         <v>42</v>
       </c>
@@ -4001,7 +4061,7 @@
         <v>31.2</v>
       </c>
     </row>
-    <row r="96" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A96" s="5" t="s">
         <v>43</v>
       </c>
@@ -4066,7 +4126,7 @@
         <v>9.8999999463558197E-2</v>
       </c>
     </row>
-    <row r="97" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A97" s="5" t="s">
         <v>44</v>
       </c>
@@ -4131,7 +4191,7 @@
         <v>1.119999960064888E-2</v>
       </c>
     </row>
-    <row r="98" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A98" s="5" t="s">
         <v>45</v>
       </c>
@@ -4196,7 +4256,7 @@
         <v>9.3800000846385956E-2</v>
       </c>
     </row>
-    <row r="99" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A99" s="5" t="s">
         <v>46</v>
       </c>
@@ -4261,7 +4321,7 @@
         <v>0.11580000072717667</v>
       </c>
     </row>
-    <row r="100" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A100" s="5" t="s">
         <v>47</v>
       </c>
@@ -4326,7 +4386,7 @@
         <v>8.959999680519104E-2</v>
       </c>
     </row>
-    <row r="101" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A101" s="5" t="s">
         <v>48</v>
       </c>
@@ -4391,7 +4451,7 @@
         <v>0.10499999672174454</v>
       </c>
     </row>
-    <row r="102" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A102" s="5" t="s">
         <v>49</v>
       </c>
@@ -4456,12 +4516,12 @@
         <v>9.0700000524520874E-2</v>
       </c>
     </row>
-    <row r="104" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="105" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A105" s="5" t="s">
         <v>53</v>
       </c>
@@ -4525,8 +4585,23 @@
       <c r="U105" s="5">
         <v>20</v>
       </c>
-    </row>
-    <row r="106" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V105" s="5">
+        <v>21</v>
+      </c>
+      <c r="W105" s="5">
+        <v>22</v>
+      </c>
+      <c r="X105" s="5">
+        <v>23</v>
+      </c>
+      <c r="Y105" s="5">
+        <v>24</v>
+      </c>
+      <c r="Z105" s="5">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="106" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A106" s="5" t="s">
         <v>41</v>
       </c>
@@ -4591,7 +4666,7 @@
         <v>11400.1</v>
       </c>
     </row>
-    <row r="107" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A107" s="5" t="s">
         <v>42</v>
       </c>
@@ -4656,7 +4731,7 @@
         <v>31.2</v>
       </c>
     </row>
-    <row r="108" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A108" s="5" t="s">
         <v>43</v>
       </c>
@@ -4721,7 +4796,7 @@
         <v>0.10019999742507935</v>
       </c>
     </row>
-    <row r="109" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A109" s="5" t="s">
         <v>44</v>
       </c>
@@ -4786,7 +4861,7 @@
         <v>7.4000000022351742E-3</v>
       </c>
     </row>
-    <row r="110" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A110" s="5" t="s">
         <v>45</v>
       </c>
@@ -4851,7 +4926,7 @@
         <v>0.10559999942779541</v>
       </c>
     </row>
-    <row r="111" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A111" s="5" t="s">
         <v>46</v>
       </c>
@@ -4916,7 +4991,7 @@
         <v>0.10909999907016754</v>
       </c>
     </row>
-    <row r="112" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A112" s="5" t="s">
         <v>47</v>
       </c>
@@ -4981,7 +5056,7 @@
         <v>9.0199999511241913E-2</v>
       </c>
     </row>
-    <row r="113" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A113" s="5" t="s">
         <v>48</v>
       </c>
@@ -5046,7 +5121,7 @@
         <v>9.8499998450279236E-2</v>
       </c>
     </row>
-    <row r="114" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A114" s="5" t="s">
         <v>49</v>
       </c>
@@ -5111,12 +5186,12 @@
         <v>9.7499996423721313E-2</v>
       </c>
     </row>
-    <row r="116" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="117" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A117" s="5" t="s">
         <v>54</v>
       </c>
@@ -5180,8 +5255,23 @@
       <c r="U117" s="5">
         <v>20</v>
       </c>
-    </row>
-    <row r="118" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V117" s="5">
+        <v>21</v>
+      </c>
+      <c r="W117" s="5">
+        <v>22</v>
+      </c>
+      <c r="X117" s="5">
+        <v>23</v>
+      </c>
+      <c r="Y117" s="5">
+        <v>24</v>
+      </c>
+      <c r="Z117" s="5">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="118" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A118" s="5" t="s">
         <v>41</v>
       </c>
@@ -5246,7 +5336,7 @@
         <v>11400.1</v>
       </c>
     </row>
-    <row r="119" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A119" s="5" t="s">
         <v>42</v>
       </c>
@@ -5311,7 +5401,7 @@
         <v>31.2</v>
       </c>
     </row>
-    <row r="120" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A120" s="5" t="s">
         <v>43</v>
       </c>
@@ -5376,7 +5466,7 @@
         <v>0.10239999741315842</v>
       </c>
     </row>
-    <row r="121" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A121" s="5" t="s">
         <v>44</v>
       </c>
@@ -5441,7 +5531,7 @@
         <v>1.2799999676644802E-2</v>
       </c>
     </row>
-    <row r="122" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A122" s="5" t="s">
         <v>45</v>
       </c>
@@ -5506,7 +5596,7 @@
         <v>0.10050000250339508</v>
       </c>
     </row>
-    <row r="123" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A123" s="5" t="s">
         <v>46</v>
       </c>
@@ -5571,7 +5661,7 @@
         <v>0.10899999737739563</v>
       </c>
     </row>
-    <row r="124" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A124" s="5" t="s">
         <v>47</v>
       </c>
@@ -5636,7 +5726,7 @@
         <v>9.1899998486042023E-2</v>
       </c>
     </row>
-    <row r="125" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A125" s="5" t="s">
         <v>48</v>
       </c>
@@ -5701,7 +5791,7 @@
         <v>0.12080000340938568</v>
       </c>
     </row>
-    <row r="126" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A126" s="5" t="s">
         <v>49</v>
       </c>

</xml_diff>